<commit_message>
Added Legislation and Word Count
</commit_message>
<xml_diff>
--- a/Idaho Cities.xlsx
+++ b/Idaho Cities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxtanous/python/influence_energy_problem/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D9BB3F3-C856-B346-9062-0F8EEB580849}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B04DE101-F556-504A-864D-C460FB6184AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40160" yWindow="3720" windowWidth="32720" windowHeight="19740" activeTab="1" xr2:uid="{143134BB-1095-B343-847D-7ABF0E2C8D6A}"/>
+    <workbookView xWindow="46520" yWindow="3520" windowWidth="32720" windowHeight="19740" activeTab="1" xr2:uid="{143134BB-1095-B343-847D-7ABF0E2C8D6A}"/>
   </bookViews>
   <sheets>
     <sheet name="CityName" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
   <si>
     <t>Boise</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>Meridian</t>
+  </si>
+  <si>
+    <t>Lewiston</t>
   </si>
 </sst>
 </file>
@@ -694,15 +697,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F28BA0E8-3EAC-F345-9F95-F28C72CED416}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -739,8 +742,11 @@
       <c r="L1" s="7" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M1" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>43.615000000000002</v>
       </c>
@@ -777,8 +783,11 @@
       <c r="L2" s="7">
         <v>43.612099999999998</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M2" s="7">
+        <v>46.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>116.20229999999999</v>
       </c>
@@ -814,6 +823,9 @@
       </c>
       <c r="L3" s="7">
         <v>116.39149999999999</v>
+      </c>
+      <c r="M3" s="7">
+        <v>117.001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>